<commit_message>
missing duc01 20inter runs
</commit_message>
<xml_diff>
--- a/bert_results.xlsx
+++ b/bert_results.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/es1595/Documents/GPPRL-DocSum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB65C4AF-A17C-FA43-8FD2-B1EC533D055B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE9DFFF-5A42-594A-B0B5-5FF87FF16B1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="460" windowWidth="14840" windowHeight="16540" xr2:uid="{D2F5A5EA-A4C2-9447-99A7-3DF95486B447}"/>
+    <workbookView xWindow="160" yWindow="460" windowWidth="17560" windowHeight="16540" xr2:uid="{D2F5A5EA-A4C2-9447-99A7-3DF95486B447}"/>
   </bookViews>
   <sheets>
-    <sheet name="cQA" sheetId="1" r:id="rId1"/>
-    <sheet name="summarisation_100" sheetId="4" r:id="rId2"/>
-    <sheet name="summarisation_20" sheetId="3" r:id="rId3"/>
-    <sheet name="summarisation_plot" sheetId="5" r:id="rId4"/>
+    <sheet name="cQA plot" sheetId="7" r:id="rId1"/>
+    <sheet name="cQA" sheetId="1" r:id="rId2"/>
+    <sheet name="summarisation_100" sheetId="4" r:id="rId3"/>
+    <sheet name="summarisation_20" sheetId="3" r:id="rId4"/>
+    <sheet name="summarisation_plot" sheetId="5" r:id="rId5"/>
+    <sheet name="summarisation_10" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="27">
   <si>
     <t>Apple</t>
   </si>
@@ -102,6 +104,21 @@
   </si>
   <si>
     <t>BERTcQA</t>
+  </si>
+  <si>
+    <t>SUPERT</t>
+  </si>
+  <si>
+    <t>NDCG at 5</t>
+  </si>
+  <si>
+    <t>Bert cQA</t>
+  </si>
+  <si>
+    <t>SUM over topics</t>
+  </si>
+  <si>
+    <t>MEAN over topics</t>
   </si>
 </sst>
 </file>
@@ -164,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,6 +189,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -486,11 +506,307 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB589FA1-118F-9E43-AAC5-DD39C3110981}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>5</v>
+      </c>
+      <c r="E1">
+        <v>10</v>
+      </c>
+      <c r="F1">
+        <v>15</v>
+      </c>
+      <c r="G1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="3">
+        <f>0.579579017169069+0.624571590523522+0.689468814723942</f>
+        <v>1.893619422416533</v>
+      </c>
+      <c r="D2" s="3">
+        <f>0.579579017169069+0.624571590523522+0.689468814723942</f>
+        <v>1.893619422416533</v>
+      </c>
+      <c r="E2" s="3">
+        <f>0.579579017169069+0.624571590523522+0.689468814723942</f>
+        <v>1.893619422416533</v>
+      </c>
+      <c r="F2" s="3">
+        <f>0.579579017169069+0.624571590523522+0.689468814723942</f>
+        <v>1.893619422416533</v>
+      </c>
+      <c r="G2" s="3">
+        <f>0.579579017169069+0.624571590523522+0.689468814723942</f>
+        <v>1.893619422416533</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6">
+        <f>0.636672184559355+0.675979195671749+0.625578036972122</f>
+        <v>1.9382294172032262</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6">
+        <f>0.580060845125319+0.583055757303753+0.617776302367445</f>
+        <v>1.780892904796517</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6">
+        <f>0.592987287762163+0.593877711677839+0.656663977017173</f>
+        <v>1.8435289764571752</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6">
+        <f>0.526259231443086+0.559194554341878+0.552389505390854</f>
+        <v>1.6378432911758178</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="6">
+        <f>0.590784755017865+0.590552934305572+0.647021827237129</f>
+        <v>1.8283595165605662</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6">
+        <f>0.714742042281167+0.730692093706664+0.743910606285843</f>
+        <v>2.1893447422736738</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5">
+        <f>C2/3</f>
+        <v>0.63120647413884434</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" ref="D10:G10" si="0">D2/3</f>
+        <v>0.63120647413884434</v>
+      </c>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63120647413884434</v>
+      </c>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63120647413884434</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="0"/>
+        <v>0.63120647413884434</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" ref="C11:G11" si="1">C3/3</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.64607647240107535</v>
+      </c>
+      <c r="F11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" ref="C12:G12" si="2">C4/3</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <f t="shared" si="2"/>
+        <v>0.59363096826550565</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" ref="C13:G13" si="3">C5/3</f>
+        <v>0</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <f t="shared" si="3"/>
+        <v>0.61450965881905839</v>
+      </c>
+      <c r="F13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="5">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" ref="C14:G14" si="4">C6/3</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <f t="shared" si="4"/>
+        <v>0.54594776372527265</v>
+      </c>
+      <c r="F14" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G14" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" ref="C15:G15" si="5">C7/3</f>
+        <v>0.60945317218685535</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <f t="shared" si="5"/>
+        <v>0.72978158075789124</v>
+      </c>
+      <c r="F15" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G15" s="5">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F27D9179-7488-4E4A-A0A7-A139B987114B}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -544,9 +860,15 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
+      <c r="C4" s="6">
+        <v>12.9</v>
+      </c>
+      <c r="D4" s="6">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="E4" s="6">
+        <v>23.6</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -642,9 +964,15 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="5">
+        <v>0.33800000000000002</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.39800000000000002</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -699,12 +1027,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8051329A-E9FC-E845-8408-CCAF9A533596}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,116 +1061,168 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E2" s="5"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.504</v>
+      </c>
+      <c r="E3" s="5"/>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.38700000000000001</v>
+      </c>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.372</v>
+      </c>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="C7" s="8">
+        <v>0.376</v>
+      </c>
+      <c r="D7" s="8">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="E7" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="D10" s="5">
+        <v>0.624</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="C11" s="5">
+        <v>0.66100000000000003</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="5">
+        <v>0.59399999999999997</v>
+      </c>
+      <c r="D13" s="5">
+        <v>0.61699999999999999</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
+      <c r="C14" s="5">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="C15" s="5">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0.752</v>
+      </c>
+      <c r="E15" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A8" r:id="rId1" xr:uid="{5A917A8B-44E0-3A48-A0C3-5C6D0A97C992}"/>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{5A917A8B-44E0-3A48-A0C3-5C6D0A97C992}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D05BC4-661F-C345-8F4D-04E7F2BEC9FE}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -896,8 +1276,12 @@
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+      <c r="C4" s="3">
+        <v>0.35599999999999998</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.38800000000000001</v>
+      </c>
       <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -947,8 +1331,12 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
+      <c r="C11" s="3">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="D11" s="3">
+        <v>0.61699999999999999</v>
+      </c>
       <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -975,12 +1363,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB7296ED-DF8D-864F-B728-C986C77C7811}">
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1015,11 +1403,15 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="3">
+        <v>0.58499999999999996</v>
+      </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="G2" s="3">
+        <v>0.66200000000000003</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
@@ -1039,10 +1431,16 @@
         <v>4</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
+      <c r="D4" s="3">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.59499999999999997</v>
+      </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
+      <c r="G4" s="3">
+        <v>0.59399999999999997</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
@@ -1052,19 +1450,191 @@
       <c r="D5" s="3"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
+      <c r="G5" s="3">
+        <v>0.61099999999999999</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="3"/>
+      <c r="C6" s="3">
+        <v>0.59799999999999998</v>
+      </c>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="3">
+        <v>0.72299999999999998</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B1FAB6-3E38-B94C-91A3-0F2D2630DDA5}">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="7"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3">
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A9" r:id="rId1" xr:uid="{3A27FA6D-935C-914B-81C8-3EE4A73C6ED2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
rerun last 2004 eig
</commit_message>
<xml_diff>
--- a/bert_results.xlsx
+++ b/bert_results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/es1595/Documents/GPPRL-DocSum/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBBC1FB0-B6FB-C34B-B35E-6031AD6141EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717B17C8-19A7-2742-A43D-3AE6804B86C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14860" windowHeight="16540" firstSheet="2" activeTab="3" xr2:uid="{D2F5A5EA-A4C2-9447-99A7-3DF95486B447}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14460" windowHeight="13460" firstSheet="1" activeTab="3" xr2:uid="{D2F5A5EA-A4C2-9447-99A7-3DF95486B447}"/>
   </bookViews>
   <sheets>
     <sheet name="cQA plot" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="38">
   <si>
     <t>Apple</t>
   </si>
@@ -132,6 +132,27 @@
   </si>
   <si>
     <t>NDCG@5</t>
+  </si>
+  <si>
+    <t>idea to improve ran gpplhh --&gt; it was previously much stronger than BT random but now weaker.</t>
+  </si>
+  <si>
+    <t>use PCA to distill the embedding to 300 dimensions?</t>
+  </si>
+  <si>
+    <t>try factor analysis</t>
+  </si>
+  <si>
+    <t>supert has embeddings with 1024 dimensions</t>
+  </si>
+  <si>
+    <t>reaper has 205?</t>
+  </si>
+  <si>
+    <t>bertcqa has 768</t>
+  </si>
+  <si>
+    <t>coala has variable number but around 50</t>
   </si>
 </sst>
 </file>
@@ -217,15 +238,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -584,7 +605,7 @@
         <f>0.58+0.625+0.689</f>
         <v>1.8940000000000001</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <f>I2+J2+K2</f>
         <v>1.893619422416533</v>
       </c>
@@ -596,13 +617,13 @@
         <f>0.58+0.625+0.689</f>
         <v>1.8940000000000001</v>
       </c>
-      <c r="I2" s="12">
+      <c r="I2" s="11">
         <v>0.57957901716906901</v>
       </c>
-      <c r="J2" s="12">
+      <c r="J2" s="11">
         <v>0.62457159052352196</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="11">
         <v>0.68946881472394195</v>
       </c>
     </row>
@@ -613,21 +634,21 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="5">
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="4">
         <f>I3+J3+K3</f>
         <v>1.9382294172032259</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-      <c r="I3" s="12">
+      <c r="I3" s="11">
         <v>0.625578036972122</v>
       </c>
-      <c r="J3" s="12">
+      <c r="J3" s="11">
         <v>0.63667218455935504</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>0.67597919567174902</v>
       </c>
     </row>
@@ -635,21 +656,21 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="5">
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="4">
         <f>I4+J4+K4</f>
         <v>1.780892904796517</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-      <c r="I4" s="12">
+      <c r="I4" s="11">
         <v>0.58006084512531897</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="11">
         <v>0.58305575730375303</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>0.61777630236744496</v>
       </c>
     </row>
@@ -660,21 +681,21 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="5">
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="4">
         <f>I5+J5+K5</f>
         <v>1.8435289764571752</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-      <c r="I5" s="12">
+      <c r="I5" s="11">
         <v>0.59298728776216303</v>
       </c>
-      <c r="J5" s="12">
+      <c r="J5" s="11">
         <v>0.59387771167783898</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>0.65666397701717305</v>
       </c>
     </row>
@@ -682,21 +703,21 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="5">
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="4">
         <f>I6+J6+K6</f>
         <v>1.6378432911758178</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-      <c r="I6" s="12">
+      <c r="I6" s="11">
         <v>0.55919455434187804</v>
       </c>
-      <c r="J6" s="12">
+      <c r="J6" s="11">
         <v>0.55238950539085396</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <v>0.52625923144308595</v>
       </c>
     </row>
@@ -704,21 +725,21 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="5">
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="4">
         <f>I7+J7+K7</f>
         <v>2.1893447422736738</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-      <c r="I7" s="12">
+      <c r="I7" s="11">
         <v>0.714742042281167</v>
       </c>
-      <c r="J7" s="12">
+      <c r="J7" s="11">
         <v>0.73069209370666399</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>0.74391060628584305</v>
       </c>
     </row>
@@ -729,33 +750,33 @@
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <f>C2/3</f>
         <v>0.63133333333333341</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <f t="shared" ref="D10:G10" si="0">D2/3</f>
         <v>0.63133333333333341</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <f t="shared" si="0"/>
         <v>0.63120647413884434</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>0.63133333333333341</v>
       </c>
-      <c r="G10" s="5">
+      <c r="G10" s="4">
         <f t="shared" si="0"/>
         <v>0.63133333333333341</v>
       </c>
-      <c r="I10" s="9">
+      <c r="I10" s="8">
         <v>0.52110936405921804</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <v>0.52780556086750996</v>
       </c>
-      <c r="K10" s="9">
+      <c r="K10" s="8">
         <v>0.56990213778503396</v>
       </c>
     </row>
@@ -766,23 +787,23 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <f t="shared" ref="C11:G11" si="1">C3/3</f>
         <v>0</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <f t="shared" si="1"/>
         <v>0.64607647240107535</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G11" s="5">
+      <c r="G11" s="4">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -791,23 +812,23 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <f t="shared" ref="C12:G12" si="2">C4/3</f>
         <v>0</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <f t="shared" si="2"/>
         <v>0.59363096826550565</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="G12" s="5">
+      <c r="G12" s="4">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -819,23 +840,23 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <f t="shared" ref="C13:G13" si="3">C5/3</f>
         <v>0</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <f t="shared" si="3"/>
         <v>0.61450965881905839</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="G13" s="5">
+      <c r="G13" s="4">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
@@ -844,23 +865,23 @@
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <f t="shared" ref="C14:G14" si="4">C6/3</f>
         <v>0</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <f t="shared" si="4"/>
         <v>0.54594776372527265</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G14" s="5">
+      <c r="G14" s="4">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
@@ -869,57 +890,57 @@
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <f t="shared" ref="C15:G15" si="5">C7/3</f>
         <v>0</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <f t="shared" si="5"/>
         <v>0.72978158075789124</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="G15" s="5">
+      <c r="G15" s="4">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <v>0.58359175791328199</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <v>0.59036683817240898</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="8">
         <v>0.63030056572253901</v>
       </c>
     </row>
     <row r="24" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <v>0.62084725450304901</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>0.62924681246354697</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="8">
         <v>0.67024588977032795</v>
       </c>
     </row>
     <row r="31" spans="9:11" x14ac:dyDescent="0.2">
-      <c r="I31" s="9">
+      <c r="I31" s="8">
         <v>0.625578036972122</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <v>0.63667218455935504</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="8">
         <v>0.67597919567174902</v>
       </c>
     </row>
@@ -933,7 +954,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:E24"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,13 +977,13 @@
       <c r="A2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="5">
         <v>40.1</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="5">
         <v>50.3</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>62</v>
       </c>
     </row>
@@ -973,13 +994,13 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>17</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>22.8</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>31.5</v>
       </c>
     </row>
@@ -987,13 +1008,13 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>12.9</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>18.100000000000001</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>23.6</v>
       </c>
     </row>
@@ -1004,13 +1025,13 @@
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>40.700000000000003</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>51</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>63.1</v>
       </c>
     </row>
@@ -1018,13 +1039,13 @@
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>8</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>14</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>9.5</v>
       </c>
     </row>
@@ -1032,13 +1053,13 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>61.4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>72.2</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>79.2</v>
       </c>
     </row>
@@ -1060,13 +1081,13 @@
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.48899999999999999</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.56499999999999995</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.66900000000000004</v>
       </c>
       <c r="G10" t="s">
@@ -1080,13 +1101,13 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0.38200000000000001</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0.40699999999999997</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>0.46700000000000003</v>
       </c>
     </row>
@@ -1094,13 +1115,13 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.33800000000000002</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.36099999999999999</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>0.39800000000000002</v>
       </c>
     </row>
@@ -1111,45 +1132,59 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.53800000000000003</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.59499999999999997</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>0.68899999999999995</v>
+      </c>
+      <c r="G13" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.309</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.32500000000000001</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.28999999999999998</v>
+      </c>
+      <c r="G14" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.73799999999999999</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.79700000000000004</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>0.84499999999999997</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G15" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>30</v>
       </c>
@@ -1162,94 +1197,103 @@
       <c r="E18" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>0.57957901716906901</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>0.62457159052352196</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="4">
         <v>0.68946881472394195</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>3</v>
       </c>
       <c r="B20" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="5">
+      <c r="C20" s="4">
         <v>0.625578036972122</v>
       </c>
-      <c r="D20" s="5">
+      <c r="D20" s="4">
         <v>0.63667218455935504</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="4">
         <v>0.67597919567174902</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>5</v>
       </c>
-      <c r="C21" s="5">
+      <c r="C21" s="4">
         <v>0.58006084512531897</v>
       </c>
-      <c r="D21" s="5">
+      <c r="D21" s="4">
         <v>0.58305575730375303</v>
       </c>
-      <c r="E21" s="5">
+      <c r="E21" s="4">
         <v>0.61777630236744496</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="G21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="5">
+      <c r="C22" s="4">
         <v>0.59298728776216303</v>
       </c>
-      <c r="D22" s="5">
+      <c r="D22" s="4">
         <v>0.59387771167783898</v>
       </c>
-      <c r="E22" s="5">
+      <c r="E22" s="4">
         <v>0.65666397701717305</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="5">
+      <c r="C23" s="4">
         <v>0.55919455434187804</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="4">
         <v>0.55238950539085396</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="4">
         <v>0.52625923144308595</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>8</v>
       </c>
-      <c r="C24" s="5">
+      <c r="C24" s="4">
         <v>0.714742042281167</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="4">
         <v>0.73069209370666399</v>
       </c>
-      <c r="E24" s="5">
+      <c r="E24" s="4">
         <v>0.74391060628584305</v>
       </c>
     </row>
@@ -1267,7 +1311,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1299,13 +1343,13 @@
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.4</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>0.438</v>
       </c>
     </row>
@@ -1316,13 +1360,13 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.46600000000000003</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.504</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.54304835906915805</v>
       </c>
     </row>
@@ -1330,13 +1374,13 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="6">
         <v>0.42035437253439101</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="6">
         <v>0.45333034238763298</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="6">
         <v>0.494892561523462</v>
       </c>
     </row>
@@ -1347,37 +1391,39 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="6">
         <v>0.35499999999999998</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>0.38700000000000001</v>
       </c>
-      <c r="E5" s="11"/>
+      <c r="E5" s="6">
+        <v>0.415437839539544</v>
+      </c>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="6">
         <v>0.372</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="6">
         <v>0.41464627033698498</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="6">
         <v>0.376</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>0.40699999999999997</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="6">
         <v>0.44699304316347199</v>
       </c>
     </row>
@@ -1390,13 +1436,13 @@
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.53900000000000003</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.624</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.65704808848596397</v>
       </c>
     </row>
@@ -1407,13 +1453,13 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0.66100000000000003</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0.69599999999999995</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>0.72745801252014097</v>
       </c>
     </row>
@@ -1421,13 +1467,13 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.63389590128379103</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.65570439601444297</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>0.67781464102100897</v>
       </c>
     </row>
@@ -1438,37 +1484,39 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.59399999999999997</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.61699999999999999</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="4">
+        <v>0.64347617049302497</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.61099999999999999</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.64688603008134404</v>
       </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.72799999999999998</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.752</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>0.76908065330195496</v>
       </c>
     </row>
@@ -1485,7 +1533,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,9 +1562,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
+      <c r="C2" s="4">
+        <v>0.26244009190401002</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1525,13 +1575,13 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.27224277444956602</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.28741446247832803</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.33293859051449898</v>
       </c>
     </row>
@@ -1539,13 +1589,13 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.27979526548911998</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.30310074854553798</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.34151216770999798</v>
       </c>
     </row>
@@ -1556,62 +1606,70 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.282204309541774</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.28825124578102101</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4">
+        <v>0.32288775243268197</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.19196380178406999</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.22031885318410199</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="4">
+        <v>0.24502677138826601</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.23171877131464599</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.25239801295768999</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="4">
+        <v>0.266877630910134</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="4">
         <v>0.26460596917576501</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>0.27973000006479298</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="4">
+        <v>0.31223049421207599</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="4">
         <v>0.206417259638558</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>0.26466108589851001</v>
       </c>
-      <c r="E9" s="5">
-        <v>0.34108803917743202</v>
+      <c r="E9" s="4">
+        <v>0.24441913145538399</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -1621,9 +1679,11 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
+      <c r="C12" s="4">
+        <v>0.53902522226552396</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -1632,13 +1692,13 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.56954875268373695</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.59572701455347299</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="4">
         <v>0.62738663553382901</v>
       </c>
     </row>
@@ -1646,13 +1706,13 @@
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.578074006291735</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.61012277019111905</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.63747967232613401</v>
       </c>
     </row>
@@ -1663,62 +1723,70 @@
       <c r="B15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.56684536007721298</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.58699237184387798</v>
       </c>
-      <c r="E15" s="5"/>
+      <c r="E15" s="4">
+        <v>0.60646722093420902</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="4">
         <v>0.54955756726098104</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="4">
         <v>0.58211283574804695</v>
       </c>
-      <c r="E16" s="5"/>
+      <c r="E16" s="4">
+        <v>0.59888257299895398</v>
+      </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>0.58443029566517202</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>0.59972568302521101</v>
       </c>
-      <c r="E17" s="5"/>
+      <c r="E17" s="4">
+        <v>0.603261819363758</v>
+      </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="4">
         <v>0.58202113647734</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>0.60806663612449197</v>
       </c>
-      <c r="E18" s="5"/>
+      <c r="E18" s="4">
+        <v>0.63288599605217399</v>
+      </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="4">
         <v>0.58364309876048703</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D19" s="4">
         <v>0.62298646981242001</v>
       </c>
-      <c r="E19" s="5">
-        <v>0.675111653403629</v>
+      <c r="E19" s="4">
+        <v>0.62134377423375398</v>
       </c>
     </row>
   </sheetData>
@@ -1734,7 +1802,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1763,13 +1831,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.4</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>0.438</v>
       </c>
     </row>
@@ -1780,13 +1848,13 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.38265604511128298</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.407585731976217</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.44770045691300703</v>
       </c>
     </row>
@@ -1794,13 +1862,13 @@
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>0.27671172048570403</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>0.28731793199689998</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.334076728640677</v>
       </c>
     </row>
@@ -1811,25 +1879,27 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>0.35599999999999998</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>0.38800000000000001</v>
       </c>
-      <c r="E5" s="10"/>
+      <c r="E5" s="4">
+        <v>0.417088270481066</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.252</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.29699999999999999</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.32145667827670099</v>
       </c>
     </row>
@@ -1837,13 +1907,13 @@
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="4">
         <v>0.29641283040869598</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>0.28361854988658902</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="4">
         <v>0.33891189187679999</v>
       </c>
     </row>
@@ -1854,13 +1924,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="C10" s="5">
+      <c r="C10" s="4">
         <v>0.53900000000000003</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="4">
         <v>0.624</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="4">
         <v>0.65704808848596397</v>
       </c>
     </row>
@@ -1871,13 +1941,13 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="4">
         <v>0.603428260871539</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="4">
         <v>0.62959627315478195</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="4">
         <v>0.66067456050143303</v>
       </c>
     </row>
@@ -1885,13 +1955,13 @@
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="4">
         <v>0.54977654820822597</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="4">
         <v>0.56135752127169602</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="4">
         <v>0.58846656400290298</v>
       </c>
     </row>
@@ -1902,25 +1972,27 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="4">
         <v>0.59499999999999997</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>0.61699999999999999</v>
       </c>
-      <c r="E13" s="10"/>
+      <c r="E13" s="4">
+        <v>0.64450020715659295</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="4">
         <v>0.52100000000000002</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="4">
         <v>0.56144000000000005</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="4">
         <v>0.57047379762068895</v>
       </c>
     </row>
@@ -1928,13 +2000,13 @@
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="4">
         <v>0.62610374400876401</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="4">
         <v>0.63045224624526897</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="4">
         <v>0.65255845301354198</v>
       </c>
     </row>
@@ -1951,7 +2023,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1986,19 +2058,19 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>0.58499999999999996</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>0.603428260871539</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>0.63200000000000001</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>0.64800000000000002</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>0.66200000000000003</v>
       </c>
     </row>
@@ -2006,19 +2078,19 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>0.53576084336504404</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>0.54977654820822597</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>0.578929580943224</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>0.60811610508432301</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="4">
         <v>0.63389590128379103</v>
       </c>
     </row>
@@ -2029,17 +2101,19 @@
       <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="10"/>
-      <c r="D4" s="5">
+      <c r="C4" s="4">
+        <v>0.59470873555191694</v>
+      </c>
+      <c r="D4" s="4">
         <v>0.59499999999999997</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>0.59499999999999997</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>0.59440187705930503</v>
       </c>
-      <c r="G4" s="5">
+      <c r="G4" s="4">
         <v>0.59399999999999997</v>
       </c>
     </row>
@@ -2047,17 +2121,19 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="5">
+      <c r="C5" s="4">
+        <v>0.53931715806045399</v>
+      </c>
+      <c r="D5" s="4">
         <v>0.52147611111874104</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>0.574302146043706</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>0.60296359702771296</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="4">
         <v>0.61099999999999999</v>
       </c>
     </row>
@@ -2065,19 +2141,19 @@
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>0.59799999999999998</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>0.62610374400876401</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>0.66152871505107702</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>0.71687539408356604</v>
       </c>
-      <c r="G6" s="5">
+      <c r="G6" s="4">
         <v>0.72299999999999998</v>
       </c>
     </row>
@@ -2091,7 +2167,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2123,11 +2199,15 @@
       <c r="A2" t="s">
         <v>22</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="4">
         <v>0.26200000000000001</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="D2" s="4">
+        <v>0.39848356289076697</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0.43849799103866299</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2136,19 +2216,23 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="4">
         <v>0.35499999999999998</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
+      <c r="D3" s="4">
+        <v>0.37559127731096797</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0.41403497636523601</v>
+      </c>
     </row>
     <row r="4" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -2157,42 +2241,58 @@
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
     </row>
     <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
     </row>
     <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>0.29199999999999998</v>
       </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="D7" s="6">
+        <v>0.29917641548857699</v>
+      </c>
+      <c r="E7" s="6">
+        <v>0.33418101337530598</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C9" s="12"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="4">
         <v>0.53900000000000003</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="D10" s="4">
+        <v>0.62144804949770205</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.65704808848596397</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2201,19 +2301,23 @@
       <c r="B11" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="4">
         <v>0.58499999999999996</v>
       </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="4">
+        <v>0.60565878617753999</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.63834532318687398</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
@@ -2222,27 +2326,31 @@
       <c r="B13" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="4">
         <v>0.59799999999999998</v>
       </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="D15" s="4">
+        <v>0.60363920104067703</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.63159688467212904</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>